<commit_message>
Update Prequal Task List - 21'04.xlsx
</commit_message>
<xml_diff>
--- a/Prequal Task List - 21'04.xlsx
+++ b/Prequal Task List - 21'04.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Git-hub.com Clone\Springboot-Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50F41E1-7187-410F-9A83-A4648885DBDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21516409-316B-4671-AEE7-7195BC548445}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="21924" windowHeight="12012" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2484" yWindow="660" windowWidth="20544" windowHeight="11136" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Auto CW " sheetId="1" r:id="rId1"/>
-    <sheet name="Tasks" sheetId="2" r:id="rId2"/>
+    <sheet name="Issues" sheetId="2" r:id="rId2"/>
+    <sheet name="Tasks" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
   <si>
     <t>Task</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -433,12 +434,416 @@
     <t xml:space="preserve">Short-term: </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t xml:space="preserve">Dao </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FacTagData Loader stopped from 3/19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>MQSI\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>林聖凱</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Action</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Follow-ups</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System Issue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Need to create FacTagData monitor.
+1. Dao data loader </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>失敗預防機制</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+2. AP </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>端預防機制</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FacTagData monitor.
+1. Dao data loader </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>失敗預防機制</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+2. AP </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>端預防機制</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. MQSI\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>林聖凱</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+2. IEAD\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>翁毓謙</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4/15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>聖凱</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> restarted loader on 4/15</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>F18P3 Lorry PreQual</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>從</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>4/12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>開始未啟動</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Need to create data quality monitor. 
+1. Bluebook</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">資料完整度
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>廠務換料</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> vs. ees-data quality
+3. AP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>端預防機制</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Bluebook 2.0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>改版</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>影響</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ees-dao</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>未能拿到</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>F18P3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>換料紀錄</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. MQSI\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>陳建良</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+2. MQSI\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>陳建良</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+3. IEAD\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>翁毓謙</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Open</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,6 +875,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
     </font>
@@ -509,7 +921,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -539,6 +951,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -886,10 +1304,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{342071F4-8D9A-43BE-9DE4-7BBB6518F8B9}">
-  <dimension ref="C3:H5"/>
+  <dimension ref="C3:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -952,6 +1370,145 @@
         <v>22</v>
       </c>
     </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="E6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98BF9A19-A3A1-4D84-9DF2-2DA0AFE2E091}">
+  <dimension ref="C3:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="5.375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="11.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.375" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.375" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="7"/>
+    <col min="9" max="9" width="36.125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="32.75" style="7" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" ht="44.4" x14ac:dyDescent="0.3">
+      <c r="C4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" ht="44.4" x14ac:dyDescent="0.3">
+      <c r="C5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" ht="59.4" x14ac:dyDescent="0.3">
+      <c r="C6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" ht="59.4" x14ac:dyDescent="0.3">
+      <c r="C7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>